<commit_message>
add enemies to canvas
</commit_message>
<xml_diff>
--- a/sharkie-parenting.xlsx
+++ b/sharkie-parenting.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sebastian Bünz\Desktop\IT\Developer Academy\Modul 12 - Sharkie\Sharkie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A80BC9C7-829A-445A-B4AB-7840F06DF538}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{095369A0-7F65-49D8-96DE-102DA903E645}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D5E54481-D8EA-4B2F-82FF-AE8F788B6374}"/>
+    <workbookView xWindow="-26955" yWindow="2370" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{D5E54481-D8EA-4B2F-82FF-AE8F788B6374}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="41">
   <si>
     <t>Klasse</t>
   </si>
@@ -134,6 +134,21 @@
   </si>
   <si>
     <t>ImageSrc</t>
+  </si>
+  <si>
+    <t>anzahl an new Enemies inh. Array = random</t>
+  </si>
+  <si>
+    <t>1.</t>
+  </si>
+  <si>
+    <t>2.</t>
+  </si>
+  <si>
+    <t>3.</t>
+  </si>
+  <si>
+    <t>4.</t>
   </si>
 </sst>
 </file>
@@ -5984,8 +5999,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11217291-8553-4542-B1F9-699469C8368F}">
   <dimension ref="B1:Y29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6278,14 +6293,41 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0364DC35-4DB9-4D74-9500-05DC3BF22F16}">
-  <dimension ref="A1"/>
+  <dimension ref="C6:D9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="4" max="4" width="40" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="6" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>